<commit_message>
completed functions for anova
</commit_message>
<xml_diff>
--- a/media/Book1.xlsx
+++ b/media/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sigmaway\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitSharma\Documents\GitHub\statsapp\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96011D20-74CC-4FC3-A36C-CAB241CF2421}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C2CBF-7BF7-46EA-9FA2-ECC9D46F8678}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8835" xr2:uid="{019CCE45-449D-4742-AC17-9DD8DC0D95E5}"/>
   </bookViews>
@@ -110,8 +110,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -165,7 +165,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -175,10 +175,10 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,11 +514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4E9463-79BE-49A9-A688-4879734CA329}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -839,7 +842,7 @@
         <v>19.989999999999998</v>
       </c>
       <c r="G14" s="9">
-        <v>1619.1899999999998</v>
+        <v>1619.19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>